<commit_message>
Update copdock and washbrook, in progress
</commit_message>
<xml_diff>
--- a/Data/Suffolk wide Neighbourhood Plan Progress.xlsx
+++ b/Data/Suffolk wide Neighbourhood Plan Progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\nps-mapping\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suffolknet.sharepoint.com/sites/NeighbourhoodPlanning/Shared Documents/NP Progress charts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BD5427-C931-469A-BD35-CB53F7925869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1222" documentId="13_ncr:1_{32273895-DA16-4E8B-83A5-787B05C8B696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFF8BD29-A0D2-4670-8083-DECF06426DE7}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1680" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Consultation Gantt Chart" sheetId="3" r:id="rId1"/>
@@ -27,6 +27,9 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -68,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="277">
   <si>
     <t>Confirmed</t>
   </si>
@@ -241,60 +244,150 @@
     <t>Beccles (reviewed - Beccles parish only)</t>
   </si>
   <si>
+    <t xml:space="preserve">yes vote, made Sept 21  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">examination summer 2021 </t>
+  </si>
+  <si>
     <t>Bredfield</t>
   </si>
   <si>
+    <t xml:space="preserve">yes vote - made May 2021 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional Post-Reg16 consultation June 2020. Examination sept 2020. </t>
+  </si>
+  <si>
     <t>Bungay</t>
   </si>
   <si>
+    <t>deadline: June 6th</t>
+  </si>
+  <si>
+    <t xml:space="preserve">made Nov 2022 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ref to be held nov 22 </t>
+  </si>
+  <si>
+    <t>Campsea Ashe</t>
+  </si>
+  <si>
     <t>Carlton Colville</t>
   </si>
   <si>
+    <t xml:space="preserve">draft seen Aug 21 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEADLINE: May 22 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inf R16 seen Jan 23 </t>
+  </si>
+  <si>
+    <t>removal of AECOM design code following R14 coments, saw inf R16  jan 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corton </t>
+  </si>
+  <si>
     <t>Earl Soham</t>
   </si>
   <si>
     <t>Easton</t>
   </si>
   <si>
+    <t xml:space="preserve">DEADLINE: 20 MARCH 23 </t>
+  </si>
+  <si>
     <t xml:space="preserve">Framlingham </t>
   </si>
   <si>
+    <t xml:space="preserve">yes-vote/made 2017. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review: discussions start March 2021. </t>
+  </si>
+  <si>
     <t>Great Bealings</t>
   </si>
   <si>
     <t>Halesworth</t>
   </si>
   <si>
+    <t xml:space="preserve">inf: sept 21 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes vote Feb 2023 </t>
+  </si>
+  <si>
+    <t>Henstead with Hulver St</t>
+  </si>
+  <si>
     <t>Kelsale cum Carlton</t>
   </si>
   <si>
     <t>Kesgrave</t>
   </si>
   <si>
+    <t>yes vote - made May 2021</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kessingland </t>
   </si>
   <si>
+    <t>yes-vote/made 2017</t>
+  </si>
+  <si>
     <t>includes allocations</t>
   </si>
   <si>
     <t xml:space="preserve">Leiston </t>
   </si>
   <si>
+    <t xml:space="preserve">yes-vote/made 2017 </t>
+  </si>
+  <si>
+    <t>Lound with Ashby, Herringfleet and Somerleyton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adopted July 2022 </t>
+  </si>
+  <si>
     <t>Lowestoft</t>
   </si>
   <si>
+    <t xml:space="preserve">inf: july 22 </t>
+  </si>
+  <si>
     <t xml:space="preserve">Martlesham </t>
   </si>
   <si>
+    <t>yes-vote/made 2018</t>
+  </si>
+  <si>
     <t>Melton</t>
   </si>
   <si>
     <t>Mettingham, Barsham, Shipmeadow, Ringsfield &amp; Weston</t>
   </si>
   <si>
+    <t>Yes vote, made 2019</t>
+  </si>
+  <si>
     <t xml:space="preserve">Otley </t>
   </si>
   <si>
+    <t xml:space="preserve">Oulton </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ref 20/02/23 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oulton Broad (superceded) </t>
+  </si>
+  <si>
     <t>In december 2018 the original neighbourhood plan area was superceded with a revised area</t>
   </si>
   <si>
@@ -304,24 +397,57 @@
     <t>Rendlesham</t>
   </si>
   <si>
+    <t>yes-vote/made 2015</t>
+  </si>
+  <si>
+    <t>yes vote, made May 2021</t>
+  </si>
+  <si>
+    <t>examination summer 2020</t>
+  </si>
+  <si>
     <t>Rushmere St Andrew</t>
   </si>
   <si>
+    <t xml:space="preserve">deadline: june 6th </t>
+  </si>
+  <si>
+    <t xml:space="preserve">POST EXAM MODS </t>
+  </si>
+  <si>
     <t>Saxmundham</t>
   </si>
   <si>
+    <t xml:space="preserve">public hearing: 27/02/23 </t>
+  </si>
+  <si>
     <t xml:space="preserve">Shadingfield, Sotterley, Willingham and Ellough </t>
   </si>
   <si>
+    <t xml:space="preserve">adopted feb 2022 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amendments to Housing Policies Jan'21 </t>
+  </si>
+  <si>
     <t>Trimley St Mary</t>
   </si>
   <si>
+    <t xml:space="preserve">Ufford </t>
+  </si>
+  <si>
     <t>Walberswick</t>
   </si>
   <si>
+    <t xml:space="preserve">Westerfield </t>
+  </si>
+  <si>
     <t>Wenhaston with Mellis Hamlet</t>
   </si>
   <si>
+    <t xml:space="preserve">yes-vote/made july 2018 </t>
+  </si>
+  <si>
     <t>Wickham Market</t>
   </si>
   <si>
@@ -334,12 +460,24 @@
     <t>Worlingham</t>
   </si>
   <si>
+    <t>made nov 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ref Nov 22 </t>
+  </si>
+  <si>
     <t>(Diss, Raydon, Burston &amp; Shimpling, Scole = South Norfolk; Palgrave, Stuston, Brome &amp; Oakley = Mid Suffolk)</t>
   </si>
   <si>
     <t xml:space="preserve">Ashbocking </t>
   </si>
   <si>
+    <t xml:space="preserve">Bacton </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Badwell Ash &amp; Long Thurlow </t>
+  </si>
+  <si>
     <t>Battisford</t>
   </si>
   <si>
@@ -349,63 +487,204 @@
     <t>Botesdale and Rickinghall</t>
   </si>
   <si>
+    <t>Yes vote, made - Jan 2020</t>
+  </si>
+  <si>
     <t>Debenham</t>
   </si>
   <si>
+    <t xml:space="preserve">Yes vote, made march 2019 </t>
+  </si>
+  <si>
     <t>Contains allocations</t>
   </si>
   <si>
     <t xml:space="preserve">Diss and District </t>
   </si>
   <si>
+    <t xml:space="preserve">  V2: APRIL 22 ...01/08/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2nd r14 in april 2022. </t>
+  </si>
+  <si>
     <t>Drinkstone</t>
   </si>
   <si>
+    <t xml:space="preserve">Yes Vote (May 2021), adopted. </t>
+  </si>
+  <si>
     <t>Elmswell</t>
   </si>
   <si>
+    <t>inf march 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1st July 22 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inf early 2021. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes vote, made March 2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Groton </t>
+  </si>
+  <si>
     <t>Haughley</t>
   </si>
   <si>
+    <t xml:space="preserve">seeking info for review, Oct 22 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes vote, made 2019 </t>
+  </si>
+  <si>
     <t>Hoxne</t>
   </si>
   <si>
+    <t>INF: Aug/sept 2021</t>
+  </si>
+  <si>
     <t>Laxfield</t>
   </si>
   <si>
+    <t>yes vote march 2022</t>
+  </si>
+  <si>
     <t>Mendlesham</t>
   </si>
   <si>
+    <t xml:space="preserve">REVIEW march 21 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> REVIEW 01/09/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes-vote/made 2017. REVIEW: Adopted Nov 2022. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modification: Review R14 stage March'21, R16 August '21. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes-vote/made march 2022 </t>
+  </si>
+  <si>
     <t>Rethinking NP with a large urban extension</t>
   </si>
   <si>
+    <t xml:space="preserve">Old Newton &amp; Dagworth with Gipping </t>
+  </si>
+  <si>
     <t>Redgrave</t>
   </si>
   <si>
+    <t xml:space="preserve">yes vote, made July 22 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ref upcoming - may not pass???? </t>
+  </si>
+  <si>
     <t>Stowupland</t>
   </si>
   <si>
+    <t>yes vote/made 2019</t>
+  </si>
+  <si>
     <t>Stradbroke</t>
   </si>
   <si>
+    <t xml:space="preserve">yes-vote/made 2019 </t>
+  </si>
+  <si>
     <t>Thorndon</t>
   </si>
   <si>
+    <t>yes vote/made March 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">post-exam mods to LGS </t>
+  </si>
+  <si>
     <t>Thurston</t>
   </si>
   <si>
+    <t>Yes vote/made 2019</t>
+  </si>
+  <si>
     <t>Walsham Le Willows</t>
   </si>
   <si>
+    <t xml:space="preserve">EXP: after may elec </t>
+  </si>
+  <si>
+    <t>Wetheringsett (com Brockford)</t>
+  </si>
+  <si>
     <t>Wilby</t>
   </si>
   <si>
+    <t xml:space="preserve">mods post examination </t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes vote, made Oct 22 </t>
+  </si>
+  <si>
+    <t>Additional 2week consulation june/july 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Babergh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acton </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXP early april </t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes vote/made jan 2020 </t>
+  </si>
+  <si>
     <t>Assington</t>
   </si>
   <si>
+    <t xml:space="preserve">yes vote/ made march 22 </t>
+  </si>
+  <si>
+    <t>Bentley</t>
+  </si>
+  <si>
+    <t>yes vote</t>
+  </si>
+  <si>
     <t>Boxford</t>
   </si>
   <si>
+    <t xml:space="preserve">inf: spring '21 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEADLINE: april 22 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes vote, made oct 2022 </t>
+  </si>
+  <si>
+    <t>Brettenham</t>
+  </si>
+  <si>
+    <t>Bures &amp; Bures St Mary (with Braintree DC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> oct 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V2 r14 exp winter '21 </t>
+  </si>
+  <si>
+    <t>Chelmondiston(and Pin Mill )</t>
+  </si>
+  <si>
     <t>Chilton</t>
   </si>
   <si>
@@ -415,36 +694,84 @@
     <t>East Bergholt</t>
   </si>
   <si>
+    <t xml:space="preserve">preparing review/mods </t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes-vote/made 2016 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">REVIEW - 2021 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edwardstone </t>
+  </si>
+  <si>
     <t>Elmsett</t>
   </si>
   <si>
     <t>Glemsford</t>
   </si>
   <si>
+    <t>EXP</t>
+  </si>
+  <si>
+    <t>Great Walding Field</t>
+  </si>
+  <si>
     <t>Hadleigh</t>
   </si>
   <si>
+    <t xml:space="preserve">Working group was disbanded july  2017. may make a re-appearance?? </t>
+  </si>
+  <si>
     <t>Hartest</t>
   </si>
   <si>
+    <t>Reg14 (V3) jan 2021</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hitcham </t>
   </si>
   <si>
+    <t xml:space="preserve">after may elect - summer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Holbrook </t>
+  </si>
+  <si>
     <t xml:space="preserve">Lavenham </t>
   </si>
   <si>
+    <t xml:space="preserve">REVIEW: inf view 5th Oct </t>
+  </si>
+  <si>
+    <t>review process: Autumn 2022</t>
+  </si>
+  <si>
     <t>Lawshall</t>
   </si>
   <si>
+    <t xml:space="preserve">R14 review: Nov 22 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">review procress begin Oct 22. </t>
+  </si>
+  <si>
     <t>Little Cornard</t>
   </si>
   <si>
+    <t xml:space="preserve">yes vote/ made July 22 </t>
+  </si>
+  <si>
     <t xml:space="preserve">Little Waldingfield </t>
   </si>
   <si>
     <t>Leavenheath</t>
   </si>
   <si>
+    <t xml:space="preserve">yes vote/ made Oct 22 </t>
+  </si>
+  <si>
     <t>Newton</t>
   </si>
   <si>
@@ -457,439 +784,124 @@
     <t>Stutton</t>
   </si>
   <si>
+    <t xml:space="preserve">parish council website inactive/no longer exists (aug 21). Call for sites summer 21. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tattingstone </t>
+  </si>
+  <si>
+    <t xml:space="preserve">des'd July '21 </t>
+  </si>
+  <si>
     <t>Whatfield</t>
   </si>
   <si>
+    <t xml:space="preserve">Wherstead </t>
+  </si>
+  <si>
     <t>Woolverstone</t>
   </si>
   <si>
     <t>Barrow cum Denham</t>
   </si>
   <si>
+    <t xml:space="preserve">Barton Mills </t>
+  </si>
+  <si>
     <t>Barningham</t>
   </si>
   <si>
     <t>Exning</t>
   </si>
   <si>
+    <t xml:space="preserve">des'd - overlap with newmarket 2018. </t>
+  </si>
+  <si>
     <t>Freckenham</t>
   </si>
   <si>
+    <t xml:space="preserve">EXP. R14 2021 </t>
+  </si>
+  <si>
     <t>Great Barton</t>
   </si>
   <si>
+    <t xml:space="preserve">Yes Vote, made June 2021 </t>
+  </si>
+  <si>
     <t>Hargrave</t>
   </si>
   <si>
+    <t xml:space="preserve">yes vote, made july 2018 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review exp- summer '21 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horringer cum Ickworth </t>
+  </si>
+  <si>
     <t>Ixworth and Ixworth Thorpe</t>
   </si>
   <si>
+    <t xml:space="preserve">EXP nov 21 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lakenheath </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mildenhall </t>
+  </si>
+  <si>
+    <t>yes vote, made july 2020</t>
+  </si>
+  <si>
     <t>Newmarket repeated reg 14 consultation</t>
   </si>
   <si>
-    <t>Additional 2week consulation june/july 2020</t>
-  </si>
-  <si>
-    <t>yes vote, made july 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wherstead </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Additional Post-Reg16 consultation June 2020. Examination sept 2020. </t>
-  </si>
-  <si>
-    <t>Great Walding Field</t>
-  </si>
-  <si>
-    <t>Brettenham</t>
-  </si>
-  <si>
-    <t>Bentley</t>
-  </si>
-  <si>
-    <t>Reg14 (V3) jan 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Holbrook </t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes vote, made july 2018 </t>
-  </si>
-  <si>
-    <t>Wetheringsett (com Brockford)</t>
-  </si>
-  <si>
-    <t>Lound with Ashby, Herringfleet and Somerleyton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amendments to Housing Policies Jan'21 </t>
-  </si>
-  <si>
-    <t>examination summer 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes-vote/made 2017. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edwardstone </t>
-  </si>
-  <si>
-    <t xml:space="preserve">inf early 2021. </t>
-  </si>
-  <si>
-    <t>Henstead with Hulver St</t>
-  </si>
-  <si>
-    <t>yes-vote/made 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes-vote/made 2017 </t>
-  </si>
-  <si>
-    <t>yes-vote/made 2018</t>
-  </si>
-  <si>
-    <t>Yes vote, made 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oulton </t>
-  </si>
-  <si>
-    <t>yes-vote/made 2015</t>
-  </si>
-  <si>
-    <t>Yes vote, made - Jan 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes vote, made 2019 </t>
-  </si>
-  <si>
-    <t>yes vote/made 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes-vote/made 2019 </t>
-  </si>
-  <si>
-    <t>Yes vote/made 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes vote/made jan 2020 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes-vote/made 2016 </t>
+    <t xml:space="preserve">West Row </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wickhambrook </t>
+  </si>
+  <si>
+    <t xml:space="preserve">issues re hedge removal at chucrh. </t>
   </si>
   <si>
     <t xml:space="preserve">Withersfield </t>
   </si>
   <si>
-    <t xml:space="preserve">Old Newton &amp; Dagworth with Gipping </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lakenheath </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes Vote (May 2021), adopted. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review exp- summer '21 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">post-exam mods to LGS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">inf: spring '21 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXP. R14 2021 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Babergh </t>
-  </si>
-  <si>
-    <t>yes vote, made May 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examination summer 2021 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes vote - made May 2021 </t>
-  </si>
-  <si>
-    <t>yes vote - made May 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes Vote, made June 2021 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">West Row </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tattingstone </t>
-  </si>
-  <si>
-    <t xml:space="preserve">des'd July '21 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">REVIEW - 2021 </t>
-  </si>
-  <si>
     <t xml:space="preserve">Worlington </t>
   </si>
   <si>
-    <t xml:space="preserve">Yes vote, made march 2019 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes vote, made March 2020 </t>
-  </si>
-  <si>
-    <t>inf march 21</t>
-  </si>
-  <si>
-    <t>Chelmondiston(and Pin Mill )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">draft seen Aug 21 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes-vote/made july 2018 </t>
-  </si>
-  <si>
-    <t>INF: Aug/sept 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modification: Review R14 stage March'21, R16 August '21. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review: discussions start March 2021. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oulton Broad (superceded) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">des'd - overlap with newmarket 2018. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">parish council website inactive/no longer exists (aug 21). Call for sites summer 21. </t>
-  </si>
-  <si>
-    <t>Bures &amp; Bures St Mary (with Braintree DC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inf: sept 21 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Westerfield </t>
-  </si>
-  <si>
-    <t xml:space="preserve">V2 r14 exp winter '21 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXP nov 21 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acton </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wickhambrook </t>
-  </si>
-  <si>
-    <t>yes vote/made March 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes-vote/made march 2022 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes vote/ made march 22 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEADLINE: april 22 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEADLINE: May 22 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO VOTE - March 2022. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  V2: APRIL 22 ...01/08/2021</t>
-  </si>
-  <si>
-    <t>yes vote march 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2nd r14 in april 2022. </t>
-  </si>
-  <si>
-    <t>deadline: June 6th</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deadline: june 6th </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barton Mills </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ref upcoming - may not pass???? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1st July 22 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bacton </t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes vote/ made July 22 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes vote, made July 22 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">inf: july 22 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Groton </t>
-  </si>
-  <si>
-    <t xml:space="preserve">REVIEW: inf view 5th Oct </t>
-  </si>
-  <si>
-    <t>review process: Autumn 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Badwell Ash &amp; Long Thurlow </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mods post examination </t>
-  </si>
-  <si>
-    <t xml:space="preserve">seeking info for review, Oct 22 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">adopted July 2022 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">adopted feb 2022 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> REVIEW 01/09/2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REVIEW march 21 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">preparing review/mods </t>
-  </si>
-  <si>
-    <t xml:space="preserve">review procress begin Oct 22. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes vote/ made Oct 22 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes vote, made Oct 22 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes vote, made oct 2022 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Horringer cum Ickworth </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> oct 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POST EXAM MODS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ref to be held nov 22 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ref Nov 22 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes-vote/made 2017. REVIEW: Adopted Nov 2022. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">R14 review: Nov 22 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes vote, made Sept 21  </t>
-  </si>
-  <si>
-    <t>DEADLINE 10 march 23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inf R16 seen Jan 23 </t>
-  </si>
-  <si>
-    <t>removal of AECOM design code following R14 coments, saw inf R16  jan 23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ref : 02/02/23 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">made Nov 2022 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ref 20/02/23 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">public hearing: 27/02/23 </t>
-  </si>
-  <si>
-    <t>made nov 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">issues re hedge removal at chucrh. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corton </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ufford </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEADLINE: 9 MARCH 23 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEADLINE: 20 MARCH 23 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Working group was disbanded july  2017. may make a re-appearance?? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">feb '23 : re-writing, removal of allocations </t>
-  </si>
-  <si>
-    <t>EXP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXP early april </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXP: Ater may elec </t>
-  </si>
-  <si>
-    <t xml:space="preserve">after may elect - summer </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXP: after may elec </t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXP Feb??? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">exp: March? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mildenhall </t>
-  </si>
-  <si>
-    <t>Campsea Ashe</t>
-  </si>
-  <si>
-    <t>yes</t>
+    <t xml:space="preserve">EXP: After may elec </t>
+  </si>
+  <si>
+    <t xml:space="preserve">began jan '23 </t>
+  </si>
+  <si>
+    <t>proposed amendments to NP following public hearings, re remove ref to Garden Neighbourhood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEADLINE: 31 MARCH '23 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEADLINE: 26 APRIL '23 </t>
+  </si>
+  <si>
+    <t>DAEDLINE: 26 APRIL 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MARCH 23 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10 March 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEADLINE: 28 APRIL 23 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO VOTE at ref - March 2022. feb '23 : re-writing with removal of allocations </t>
   </si>
 </sst>
 </file>
@@ -1629,9 +1641,6 @@
     <xf numFmtId="17" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1642,9 +1651,6 @@
     <xf numFmtId="17" fontId="0" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1652,6 +1658,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1997,35 +2009,36 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.42578125" customWidth="1"/>
-    <col min="8" max="9" width="4.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.44140625" customWidth="1"/>
+    <col min="8" max="8" width="4.5546875" customWidth="1"/>
+    <col min="9" max="9" width="4.6640625" customWidth="1"/>
     <col min="10" max="10" width="5" customWidth="1"/>
-    <col min="11" max="11" width="5.42578125" customWidth="1"/>
-    <col min="12" max="12" width="4.42578125" customWidth="1"/>
+    <col min="11" max="11" width="5.44140625" customWidth="1"/>
+    <col min="12" max="12" width="4.33203125" customWidth="1"/>
     <col min="13" max="14" width="5" customWidth="1"/>
-    <col min="15" max="15" width="5.140625" customWidth="1"/>
-    <col min="16" max="16" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.85546875" customWidth="1"/>
-    <col min="27" max="27" width="18.42578125" customWidth="1"/>
-    <col min="28" max="28" width="21.5703125" customWidth="1"/>
-    <col min="29" max="29" width="18.140625" customWidth="1"/>
-    <col min="30" max="30" width="13.5703125" customWidth="1"/>
-    <col min="31" max="31" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="5.109375" customWidth="1"/>
+    <col min="16" max="16" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.88671875" customWidth="1"/>
+    <col min="27" max="27" width="18.44140625" customWidth="1"/>
+    <col min="28" max="28" width="21.6640625" customWidth="1"/>
+    <col min="29" max="29" width="18.109375" customWidth="1"/>
+    <col min="30" max="30" width="13.5546875" customWidth="1"/>
+    <col min="31" max="31" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
@@ -2036,7 +2049,7 @@
       <c r="E1" s="122"/>
       <c r="F1" s="122"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2046,7 +2059,7 @@
       <c r="E2" s="121"/>
       <c r="F2" s="121"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2056,8 +2069,8 @@
       <c r="E3" s="120"/>
       <c r="F3" s="120"/>
     </row>
-    <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:24" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C5" s="117" t="s">
         <v>4</v>
       </c>
@@ -2091,7 +2104,7 @@
       <c r="W5" s="118"/>
       <c r="X5" s="119"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>9</v>
       </c>
@@ -2165,7 +2178,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -2195,7 +2208,7 @@
       <c r="W7" s="23"/>
       <c r="X7" s="24"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -2225,7 +2238,7 @@
       <c r="W8" s="23"/>
       <c r="X8" s="24"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -2255,7 +2268,7 @@
       <c r="W9" s="23"/>
       <c r="X9" s="24"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -2285,7 +2298,7 @@
       <c r="W10" s="23"/>
       <c r="X10" s="24"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2315,7 +2328,7 @@
       <c r="W11" s="23"/>
       <c r="X11" s="24"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -2345,7 +2358,7 @@
       <c r="W12" s="23"/>
       <c r="X12" s="24"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -2375,7 +2388,7 @@
       <c r="W13" s="23"/>
       <c r="X13" s="24"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -2405,7 +2418,7 @@
       <c r="W14" s="32"/>
       <c r="X14" s="33"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -2435,7 +2448,7 @@
       <c r="W15" s="23"/>
       <c r="X15" s="24"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -2465,7 +2478,7 @@
       <c r="W16" s="23"/>
       <c r="X16" s="24"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -2495,7 +2508,7 @@
       <c r="W17" s="23"/>
       <c r="X17" s="24"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -2525,7 +2538,7 @@
       <c r="W18" s="23"/>
       <c r="X18" s="24"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -2555,7 +2568,7 @@
       <c r="W19" s="32"/>
       <c r="X19" s="33"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C20" s="22"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
@@ -2579,7 +2592,7 @@
       <c r="W20" s="23"/>
       <c r="X20" s="24"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C21" s="22"/>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
@@ -2603,7 +2616,7 @@
       <c r="W21" s="23"/>
       <c r="X21" s="24"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C22" s="22"/>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
@@ -2627,7 +2640,7 @@
       <c r="W22" s="23"/>
       <c r="X22" s="24"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C23" s="22"/>
       <c r="D23" s="23"/>
       <c r="E23" s="23"/>
@@ -2651,7 +2664,7 @@
       <c r="W23" s="23"/>
       <c r="X23" s="24"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C24" s="22"/>
       <c r="D24" s="23"/>
       <c r="E24" s="23"/>
@@ -2675,7 +2688,7 @@
       <c r="W24" s="23"/>
       <c r="X24" s="24"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C25" s="22"/>
       <c r="D25" s="23"/>
       <c r="E25" s="23"/>
@@ -2723,21 +2736,21 @@
   <dimension ref="A1:J129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H86" sqref="H86"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.140625" style="3" customWidth="1"/>
-    <col min="2" max="5" width="27.5703125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="47.109375" style="3" customWidth="1"/>
+    <col min="2" max="5" width="27.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="27.88671875" style="4" customWidth="1"/>
     <col min="7" max="7" width="29" style="60" customWidth="1"/>
-    <col min="8" max="8" width="82.85546875" style="4" customWidth="1"/>
-    <col min="9" max="10" width="27.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="82.88671875" style="4" customWidth="1"/>
+    <col min="9" max="10" width="27.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>45</v>
       </c>
@@ -2766,7 +2779,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>37</v>
       </c>
@@ -2779,7 +2792,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>54</v>
       </c>
@@ -2789,17 +2802,17 @@
       <c r="C3" s="6"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="111">
+      <c r="B4" s="110">
         <v>43252</v>
       </c>
       <c r="C4" s="8"/>
       <c r="G4" s="61"/>
     </row>
-    <row r="5" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>56</v>
       </c>
@@ -2809,15 +2822,15 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="85" t="s">
-        <v>248</v>
+        <v>57</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -2825,15 +2838,15 @@
       <c r="E6" s="7"/>
       <c r="F6" s="49"/>
       <c r="G6" s="49" t="s">
-        <v>181</v>
+        <v>60</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -2841,54 +2854,54 @@
         <v>44501</v>
       </c>
       <c r="E7" s="49" t="s">
-        <v>217</v>
+        <v>63</v>
       </c>
       <c r="F7" s="49"/>
       <c r="G7" s="67" t="s">
-        <v>253</v>
+        <v>64</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>272</v>
+        <v>66</v>
       </c>
       <c r="B8" s="73">
         <v>44927</v>
       </c>
       <c r="C8" s="11"/>
-      <c r="D8" s="116"/>
+      <c r="D8" s="114"/>
       <c r="E8" s="52"/>
       <c r="F8" s="52"/>
       <c r="G8" s="61"/>
     </row>
-    <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B9" s="56"/>
       <c r="C9" s="8" t="s">
-        <v>193</v>
+        <v>68</v>
       </c>
       <c r="D9" s="49" t="s">
-        <v>212</v>
-      </c>
-      <c r="E9" s="109" t="s">
-        <v>250</v>
+        <v>69</v>
+      </c>
+      <c r="E9" s="108" t="s">
+        <v>70</v>
       </c>
       <c r="F9" s="52"/>
       <c r="G9" s="61"/>
       <c r="H9" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="B10" s="112">
+        <v>72</v>
+      </c>
+      <c r="B10" s="111">
         <v>43891</v>
       </c>
       <c r="D10" s="52"/>
@@ -2896,9 +2909,9 @@
       <c r="F10" s="52"/>
       <c r="G10" s="61"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="B11" s="86">
         <v>43070</v>
@@ -2909,24 +2922,24 @@
       <c r="F11" s="52"/>
       <c r="G11" s="61"/>
     </row>
-    <row r="12" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="B12" s="73">
         <v>43070</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="D12" s="114" t="s">
-        <v>261</v>
+      <c r="D12" s="112" t="s">
+        <v>75</v>
       </c>
       <c r="E12" s="52"/>
       <c r="F12" s="52"/>
       <c r="G12" s="61"/>
     </row>
-    <row r="13" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -2934,15 +2947,15 @@
       <c r="E13" s="54"/>
       <c r="F13" s="55"/>
       <c r="G13" s="62" t="s">
-        <v>153</v>
+        <v>77</v>
       </c>
       <c r="H13" s="42" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -2950,16 +2963,16 @@
       <c r="E14" s="49"/>
       <c r="F14" s="49"/>
       <c r="G14" s="62" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7" t="s">
-        <v>202</v>
+        <v>81</v>
       </c>
       <c r="D15" s="87">
         <v>44531</v>
@@ -2968,15 +2981,15 @@
         <v>44776</v>
       </c>
       <c r="F15" s="49"/>
-      <c r="G15" s="61" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G15" s="67" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B16" s="111">
+        <v>83</v>
+      </c>
+      <c r="B16" s="110">
         <v>42614</v>
       </c>
       <c r="C16" s="8"/>
@@ -2985,11 +2998,11 @@
       <c r="F16" s="52"/>
       <c r="G16" s="61"/>
     </row>
-    <row r="17" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" s="111">
+        <v>84</v>
+      </c>
+      <c r="B17" s="110">
         <v>43040</v>
       </c>
       <c r="D17"/>
@@ -2997,9 +3010,9 @@
       <c r="F17" s="51"/>
       <c r="G17" s="63"/>
     </row>
-    <row r="18" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -3007,12 +3020,12 @@
       <c r="E18" s="6"/>
       <c r="F18" s="49"/>
       <c r="G18" s="67" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -3020,15 +3033,15 @@
       <c r="E19" s="7"/>
       <c r="F19" s="49"/>
       <c r="G19" s="64" t="s">
-        <v>157</v>
+        <v>88</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -3036,12 +3049,12 @@
       <c r="E20" s="7"/>
       <c r="F20" s="6"/>
       <c r="G20" s="65" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
-        <v>150</v>
+        <v>92</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -3053,25 +3066,25 @@
       </c>
       <c r="F21" s="49"/>
       <c r="G21" s="64" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="D22" s="113" t="s">
-        <v>260</v>
+        <v>95</v>
+      </c>
+      <c r="D22" s="43" t="s">
+        <v>273</v>
       </c>
       <c r="F22" s="52"/>
     </row>
-    <row r="23" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -3079,12 +3092,12 @@
       <c r="E23" s="46"/>
       <c r="F23" s="49"/>
       <c r="G23" s="65" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -3092,12 +3105,12 @@
       <c r="E24" s="46"/>
       <c r="F24" s="49"/>
       <c r="G24" s="65" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="B25" s="73">
         <v>43891</v>
@@ -3108,7 +3121,7 @@
       <c r="F25" s="50"/>
       <c r="G25" s="66"/>
     </row>
-    <row r="26" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>42</v>
       </c>
@@ -3118,12 +3131,12 @@
       <c r="E26" s="46"/>
       <c r="F26" s="49"/>
       <c r="G26" s="67" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="B27" s="73">
         <v>43556</v>
@@ -3134,9 +3147,9 @@
       <c r="F27" s="50"/>
       <c r="G27" s="61"/>
     </row>
-    <row r="28" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>161</v>
+        <v>102</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -3148,12 +3161,12 @@
       </c>
       <c r="F28" s="49"/>
       <c r="G28" s="61" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>198</v>
+        <v>104</v>
       </c>
       <c r="B29" s="73">
         <v>43891</v>
@@ -3164,12 +3177,12 @@
       <c r="F29" s="52"/>
       <c r="G29" s="61"/>
       <c r="H29" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="B30" s="73">
         <v>42887</v>
@@ -3180,9 +3193,9 @@
       <c r="F30" s="48"/>
       <c r="G30" s="61"/>
     </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -3190,13 +3203,13 @@
       <c r="E31" s="49"/>
       <c r="F31" s="49"/>
       <c r="G31" s="62" t="s">
-        <v>162</v>
+        <v>108</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>43</v>
       </c>
@@ -3206,15 +3219,15 @@
       <c r="E32" s="49"/>
       <c r="F32" s="106"/>
       <c r="G32" s="49" t="s">
-        <v>179</v>
+        <v>109</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -3222,16 +3235,16 @@
         <v>44501</v>
       </c>
       <c r="E33" s="49" t="s">
-        <v>218</v>
+        <v>112</v>
       </c>
       <c r="F33" s="106" t="s">
-        <v>243</v>
+        <v>113</v>
       </c>
       <c r="G33" s="61"/>
     </row>
-    <row r="34" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -3241,14 +3254,17 @@
       <c r="E34" s="100">
         <v>44806</v>
       </c>
-      <c r="F34" s="110" t="s">
-        <v>255</v>
+      <c r="F34" s="109" t="s">
+        <v>115</v>
       </c>
       <c r="G34" s="63"/>
-    </row>
-    <row r="35" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H34" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -3263,7 +3279,7 @@
       </c>
       <c r="G35" s="61"/>
     </row>
-    <row r="36" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>44</v>
       </c>
@@ -3273,15 +3289,15 @@
       <c r="E36" s="43"/>
       <c r="F36" s="76"/>
       <c r="G36" s="67" t="s">
-        <v>233</v>
+        <v>117</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="B37" s="73">
         <v>42767</v>
@@ -3291,9 +3307,9 @@
       <c r="E37" s="52"/>
       <c r="F37" s="52"/>
     </row>
-    <row r="38" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>259</v>
+        <v>120</v>
       </c>
       <c r="B38" s="73">
         <v>44652</v>
@@ -3303,9 +3319,9 @@
       <c r="E38" s="52"/>
       <c r="F38" s="52"/>
     </row>
-    <row r="39" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>82</v>
+        <v>121</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -3313,9 +3329,9 @@
       <c r="E39" s="52"/>
       <c r="F39" s="52"/>
     </row>
-    <row r="40" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>203</v>
+        <v>122</v>
       </c>
       <c r="B40" s="73">
         <v>44440</v>
@@ -3323,9 +3339,9 @@
       <c r="C40" s="73"/>
       <c r="F40" s="52"/>
     </row>
-    <row r="41" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="10" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -3333,12 +3349,12 @@
       <c r="E41" s="6"/>
       <c r="F41" s="49"/>
       <c r="G41" s="64" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="10" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -3350,21 +3366,21 @@
       </c>
       <c r="F42" s="52"/>
     </row>
-    <row r="43" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
       <c r="B43" s="73">
         <v>42125</v>
       </c>
       <c r="C43" s="7"/>
       <c r="H43" s="15" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -3376,73 +3392,73 @@
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="64" t="s">
-        <v>256</v>
+        <v>129</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="14" t="s">
         <v>31</v>
       </c>
       <c r="B46" s="77"/>
       <c r="C46" s="77"/>
     </row>
-    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>89</v>
+        <v>132</v>
       </c>
       <c r="B48" s="73">
         <v>43770</v>
       </c>
       <c r="C48" s="80"/>
     </row>
-    <row r="49" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
-        <v>222</v>
+        <v>133</v>
       </c>
       <c r="B49" s="73">
         <v>44763</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
-        <v>229</v>
+        <v>134</v>
       </c>
       <c r="B50" s="73">
         <v>44805</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="B51" s="73">
         <v>43800</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="73"/>
       <c r="D52" s="73">
         <v>44287</v>
       </c>
-      <c r="E52" s="42" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E52" s="102" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
-        <v>92</v>
+        <v>137</v>
       </c>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -3450,12 +3466,12 @@
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
       <c r="G53" s="65" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -3463,32 +3479,34 @@
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
       <c r="G54" s="65" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
       <c r="D55" s="91" t="s">
-        <v>214</v>
+        <v>143</v>
       </c>
       <c r="E55" s="86">
         <v>44896</v>
       </c>
-      <c r="F55" s="6"/>
+      <c r="F55" s="6" t="s">
+        <v>268</v>
+      </c>
       <c r="H55" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
-        <v>96</v>
+        <v>145</v>
       </c>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -3496,28 +3514,30 @@
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
       <c r="G56" s="64" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
-        <v>97</v>
+        <v>147</v>
       </c>
       <c r="B57" s="7"/>
       <c r="C57" s="7" t="s">
-        <v>191</v>
+        <v>148</v>
       </c>
       <c r="D57" s="95" t="s">
-        <v>221</v>
-      </c>
-      <c r="E57" s="11"/>
+        <v>149</v>
+      </c>
+      <c r="E57" s="115" t="s">
+        <v>271</v>
+      </c>
       <c r="F57" s="11"/>
       <c r="G57" s="68"/>
       <c r="H57" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>34</v>
       </c>
@@ -3527,10 +3547,10 @@
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
       <c r="G58" s="65" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>33</v>
       </c>
@@ -3540,12 +3560,12 @@
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
       <c r="G59" s="65" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
-        <v>226</v>
+        <v>152</v>
       </c>
       <c r="B60" s="73">
         <v>44743</v>
@@ -3556,39 +3576,39 @@
       <c r="F60" s="11"/>
       <c r="G60" s="68"/>
     </row>
-    <row r="61" spans="1:8" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="B61" s="7"/>
       <c r="C61" s="7" t="s">
-        <v>231</v>
+        <v>154</v>
       </c>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
       <c r="G61" s="65" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
-        <v>99</v>
+        <v>156</v>
       </c>
       <c r="B62" s="7"/>
       <c r="C62" s="7" t="s">
-        <v>195</v>
+        <v>157</v>
       </c>
       <c r="D62" s="91">
         <v>44593</v>
       </c>
-      <c r="E62" s="42" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E62" s="102" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
-        <v>100</v>
+        <v>158</v>
       </c>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -3596,30 +3616,30 @@
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
       <c r="G63" s="72" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="16.350000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="16.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
-        <v>101</v>
+        <v>160</v>
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7" t="s">
-        <v>235</v>
+        <v>161</v>
       </c>
       <c r="E64" s="91" t="s">
-        <v>234</v>
+        <v>162</v>
       </c>
       <c r="F64" s="49"/>
       <c r="G64" s="64" t="s">
-        <v>246</v>
+        <v>163</v>
       </c>
       <c r="H64" s="42" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>41</v>
       </c>
@@ -3629,15 +3649,15 @@
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
       <c r="G65" s="72" t="s">
-        <v>209</v>
+        <v>165</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B66" s="73">
         <v>43862</v>
@@ -3648,9 +3668,9 @@
       <c r="F66" s="52"/>
       <c r="G66" s="61"/>
     </row>
-    <row r="67" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
-        <v>103</v>
+        <v>168</v>
       </c>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -3660,15 +3680,15 @@
       </c>
       <c r="F67" s="73"/>
       <c r="G67" s="72" t="s">
-        <v>224</v>
+        <v>169</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
-        <v>104</v>
+        <v>171</v>
       </c>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -3676,12 +3696,12 @@
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
       <c r="G68" s="65" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
-        <v>105</v>
+        <v>173</v>
       </c>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -3689,15 +3709,15 @@
       <c r="E69" s="7"/>
       <c r="F69" s="7"/>
       <c r="G69" s="65" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
-        <v>106</v>
+        <v>175</v>
       </c>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -3705,15 +3725,15 @@
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
       <c r="G70" s="72" t="s">
-        <v>208</v>
+        <v>176</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
-        <v>107</v>
+        <v>178</v>
       </c>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -3721,12 +3741,12 @@
       <c r="E71" s="7"/>
       <c r="F71" s="7"/>
       <c r="G71" s="65" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
-        <v>108</v>
+        <v>180</v>
       </c>
       <c r="B72" s="73">
         <v>43282</v>
@@ -3736,12 +3756,12 @@
         <v>44896</v>
       </c>
       <c r="E72" s="42" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
-        <v>149</v>
+        <v>182</v>
       </c>
       <c r="B73" s="73">
         <v>44197</v>
@@ -3750,13 +3770,13 @@
       <c r="D73" s="86">
         <v>44774</v>
       </c>
-      <c r="E73" s="108" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E73" s="84" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
-        <v>109</v>
+        <v>183</v>
       </c>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -3764,10 +3784,10 @@
       <c r="E74" s="7"/>
       <c r="F74" s="7"/>
       <c r="G74" s="64" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>32</v>
       </c>
@@ -3776,33 +3796,33 @@
       <c r="D75" s="7"/>
       <c r="E75" s="7"/>
       <c r="F75" s="73" t="s">
-        <v>230</v>
+        <v>184</v>
       </c>
       <c r="G75" s="64" t="s">
-        <v>239</v>
+        <v>185</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="14" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="B78" s="86">
         <v>44470</v>
       </c>
       <c r="C78" s="93"/>
       <c r="D78" s="42" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>30</v>
       </c>
@@ -3812,12 +3832,12 @@
       <c r="E79" s="7"/>
       <c r="F79" s="7"/>
       <c r="G79" s="65" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
-        <v>110</v>
+        <v>191</v>
       </c>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -3827,12 +3847,12 @@
         <v>44378</v>
       </c>
       <c r="G80" s="72" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>145</v>
+        <v>193</v>
       </c>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -3844,31 +3864,31 @@
         <v>44774</v>
       </c>
       <c r="G81" s="64" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
-        <v>111</v>
+        <v>195</v>
       </c>
       <c r="B82" s="7"/>
       <c r="C82" s="7" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="D82" s="82">
         <v>44440</v>
       </c>
       <c r="E82" s="93" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="F82" s="6"/>
       <c r="G82" s="64" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
-        <v>144</v>
+        <v>199</v>
       </c>
       <c r="B83" s="73">
         <v>44197</v>
@@ -3876,29 +3896,29 @@
       <c r="C83" s="11"/>
       <c r="D83" s="74"/>
     </row>
-    <row r="84" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B84" s="73" t="s">
         <v>201</v>
-      </c>
-      <c r="B84" s="73" t="s">
-        <v>242</v>
       </c>
       <c r="C84" s="11"/>
       <c r="D84" s="74"/>
     </row>
-    <row r="85" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
       <c r="D85" s="71" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -3906,13 +3926,13 @@
       <c r="E86" s="7"/>
       <c r="F86" s="7"/>
       <c r="G86" s="85" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="H86" s="45"/>
     </row>
-    <row r="87" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
-        <v>112</v>
+        <v>204</v>
       </c>
       <c r="B87" s="73">
         <v>43070</v>
@@ -3922,58 +3942,58 @@
       <c r="E87" s="11"/>
       <c r="F87" s="11"/>
     </row>
-    <row r="88" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
-        <v>113</v>
+        <v>205</v>
       </c>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
-      <c r="D88" s="7"/>
-      <c r="E88" s="6"/>
-      <c r="F88" s="6"/>
-      <c r="G88" s="92" t="s">
-        <v>213</v>
-      </c>
-      <c r="H88" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D88" s="115" t="s">
+        <v>275</v>
+      </c>
+      <c r="E88" s="116"/>
+      <c r="F88" s="116"/>
+      <c r="G88" s="92"/>
+      <c r="H88" s="102" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
-        <v>114</v>
+        <v>206</v>
       </c>
       <c r="B89" s="7"/>
       <c r="C89" s="7" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
       <c r="D89" s="103"/>
       <c r="E89" s="103"/>
       <c r="F89" s="103"/>
       <c r="G89" s="105" t="s">
-        <v>169</v>
+        <v>208</v>
       </c>
       <c r="H89" s="42" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
-        <v>154</v>
+        <v>210</v>
       </c>
       <c r="B90" s="73">
         <v>44256</v>
       </c>
       <c r="C90" s="11"/>
       <c r="D90" s="71" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E90" s="11"/>
       <c r="F90" s="11"/>
       <c r="G90" s="68"/>
     </row>
-    <row r="91" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
-        <v>115</v>
+        <v>211</v>
       </c>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -3981,27 +4001,27 @@
       <c r="E91" s="7"/>
       <c r="F91" s="7"/>
       <c r="G91" s="69" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
-        <v>116</v>
+        <v>212</v>
       </c>
       <c r="B92" s="73">
         <v>43009</v>
       </c>
-      <c r="C92" s="115" t="s">
-        <v>264</v>
+      <c r="C92" s="113" t="s">
+        <v>213</v>
       </c>
       <c r="D92" s="45"/>
       <c r="E92" s="45"/>
       <c r="F92" s="52"/>
       <c r="G92" s="70"/>
     </row>
-    <row r="93" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
-        <v>143</v>
+        <v>214</v>
       </c>
       <c r="B93" s="73">
         <v>42917</v>
@@ -4011,21 +4031,21 @@
         <v>44774</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
-        <v>117</v>
+        <v>215</v>
       </c>
       <c r="B94" s="73">
         <v>42156</v>
       </c>
       <c r="D94" s="45"/>
       <c r="H94" s="4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
-        <v>118</v>
+        <v>217</v>
       </c>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -4033,24 +4053,24 @@
         <v>44256</v>
       </c>
       <c r="H95" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
-        <v>119</v>
+        <v>219</v>
       </c>
       <c r="B96" s="73">
         <v>43831</v>
       </c>
       <c r="C96" s="40"/>
-      <c r="D96" s="115" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D96" s="113" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
-        <v>147</v>
+        <v>221</v>
       </c>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -4061,13 +4081,13 @@
         <v>44927</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
-        <v>120</v>
+        <v>222</v>
       </c>
       <c r="B98" s="7"/>
       <c r="C98" s="7" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D98" s="86">
         <v>44958</v>
@@ -4075,33 +4095,33 @@
       <c r="E98" s="103"/>
       <c r="F98" s="103"/>
       <c r="G98" s="104" t="s">
-        <v>169</v>
+        <v>208</v>
       </c>
       <c r="H98" s="102" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
-        <v>121</v>
+        <v>225</v>
       </c>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
       <c r="D99" s="7" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
       <c r="E99" s="103"/>
       <c r="F99" s="103"/>
       <c r="G99" s="104" t="s">
-        <v>158</v>
+        <v>91</v>
       </c>
       <c r="H99" s="102" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
-        <v>122</v>
+        <v>228</v>
       </c>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -4113,12 +4133,12 @@
       </c>
       <c r="F100" s="95"/>
       <c r="G100" s="96" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
-        <v>123</v>
+        <v>230</v>
       </c>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -4126,12 +4146,12 @@
       <c r="E101" s="7"/>
       <c r="F101" s="7"/>
       <c r="G101" s="72" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
-        <v>124</v>
+        <v>231</v>
       </c>
       <c r="B102" s="7"/>
       <c r="C102" s="73">
@@ -4145,7 +4165,7 @@
       </c>
       <c r="F102" s="6"/>
     </row>
-    <row r="103" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
         <v>29</v>
       </c>
@@ -4157,12 +4177,12 @@
       </c>
       <c r="F103" s="93"/>
       <c r="G103" s="64" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
-        <v>125</v>
+        <v>233</v>
       </c>
       <c r="B104" s="7"/>
       <c r="C104" s="79"/>
@@ -4170,12 +4190,12 @@
       <c r="E104" s="7"/>
       <c r="F104" s="7"/>
       <c r="G104" s="72" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
-        <v>126</v>
+        <v>234</v>
       </c>
       <c r="B105" s="73">
         <v>43922</v>
@@ -4188,18 +4208,18 @@
         <v>44958</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
-        <v>127</v>
+        <v>235</v>
       </c>
       <c r="B106" s="73">
         <v>43070</v>
       </c>
       <c r="C106" s="77"/>
     </row>
-    <row r="107" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
-        <v>128</v>
+        <v>236</v>
       </c>
       <c r="B107" s="73">
         <v>43374</v>
@@ -4215,24 +4235,24 @@
         <v>44866</v>
       </c>
       <c r="H107" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
-        <v>185</v>
+        <v>238</v>
       </c>
       <c r="B108" s="73">
         <v>44378</v>
       </c>
       <c r="C108" s="77"/>
       <c r="H108" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
-        <v>129</v>
+        <v>240</v>
       </c>
       <c r="B109" s="7"/>
       <c r="C109" s="6"/>
@@ -4240,12 +4260,12 @@
       <c r="E109" s="7"/>
       <c r="F109" s="7"/>
       <c r="G109" s="72" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
-        <v>141</v>
+        <v>241</v>
       </c>
       <c r="B110" s="73">
         <v>44075</v>
@@ -4258,23 +4278,23 @@
         <v>44927</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
-        <v>130</v>
+        <v>242</v>
       </c>
       <c r="B111" s="73">
         <v>43374</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="14" t="s">
         <v>39</v>
       </c>
       <c r="C113" s="77"/>
     </row>
-    <row r="114" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="s">
-        <v>131</v>
+        <v>243</v>
       </c>
       <c r="B114" s="73">
         <v>43617</v>
@@ -4282,50 +4302,50 @@
       <c r="C114" s="78"/>
       <c r="D114" s="77"/>
     </row>
-    <row r="115" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="s">
-        <v>219</v>
+        <v>244</v>
       </c>
       <c r="B115" s="73">
         <v>44621</v>
       </c>
       <c r="C115" s="78"/>
     </row>
-    <row r="116" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="3" t="s">
-        <v>132</v>
+        <v>245</v>
       </c>
       <c r="B116" s="73">
         <v>42826</v>
       </c>
       <c r="C116" s="78"/>
     </row>
-    <row r="117" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="3" t="s">
-        <v>133</v>
+        <v>246</v>
       </c>
       <c r="B117" s="73">
         <v>43252</v>
       </c>
       <c r="H117" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="s">
-        <v>134</v>
+        <v>248</v>
       </c>
       <c r="B118" s="73">
         <v>43405</v>
       </c>
       <c r="C118" s="7"/>
       <c r="D118" s="42" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="3" t="s">
-        <v>135</v>
+        <v>250</v>
       </c>
       <c r="B119" s="73">
         <v>43466</v>
@@ -4335,12 +4355,12 @@
       <c r="E119" s="7"/>
       <c r="F119" s="7"/>
       <c r="G119" s="72" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="s">
-        <v>136</v>
+        <v>252</v>
       </c>
       <c r="B120" s="73">
         <v>42309</v>
@@ -4350,52 +4370,52 @@
       <c r="E120" s="7"/>
       <c r="F120" s="7"/>
       <c r="G120" s="65" t="s">
-        <v>148</v>
+        <v>253</v>
       </c>
       <c r="H120" s="42" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="3" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="B121" s="73">
         <v>44621</v>
       </c>
       <c r="C121" s="11"/>
     </row>
-    <row r="122" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="3" t="s">
-        <v>137</v>
+        <v>256</v>
       </c>
       <c r="B122" s="73">
         <v>42917</v>
       </c>
       <c r="C122" s="7"/>
       <c r="D122" s="42" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="3" t="s">
-        <v>172</v>
+        <v>258</v>
       </c>
       <c r="B123" s="73">
         <v>44228</v>
       </c>
       <c r="C123" s="11"/>
     </row>
-    <row r="124" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="3" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="B124" s="73">
         <v>44958</v>
       </c>
       <c r="C124" s="11"/>
     </row>
-    <row r="125" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="3" t="s">
         <v>40</v>
       </c>
@@ -4407,35 +4427,35 @@
       <c r="E125" s="7"/>
       <c r="F125" s="7"/>
       <c r="G125" s="65" t="s">
-        <v>140</v>
+        <v>260</v>
       </c>
       <c r="H125" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="3" t="s">
-        <v>184</v>
+        <v>262</v>
       </c>
       <c r="B126" s="73">
         <v>44317</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="3" t="s">
-        <v>207</v>
+        <v>263</v>
       </c>
       <c r="B127" s="73">
         <v>44470</v>
       </c>
       <c r="C127" s="6"/>
       <c r="H127" s="4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="3" t="s">
-        <v>170</v>
+        <v>265</v>
       </c>
       <c r="B128" s="73">
         <v>43831</v>
@@ -4445,9 +4465,9 @@
         <v>44896</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
-        <v>188</v>
+        <v>266</v>
       </c>
       <c r="B129" s="73">
         <v>44409</v>
@@ -4464,6 +4484,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="890b14a5-ed4a-422d-85a5-a10e9e237f7d">
+      <UserInfo>
+        <DisplayName>Ross Walker</DisplayName>
+        <AccountId>22</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4472,7 +4506,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001146855AE4E7AF458AFEAD9125E16BBC" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="551a0b2fae230f565607a8a48245518d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fefe685c-4b3f-4318-a1ea-8497c774326c" xmlns:ns3="890b14a5-ed4a-422d-85a5-a10e9e237f7d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e295616fe3ca5139c880945067fa21a5" ns2:_="" ns3:_="">
     <xsd:import namespace="fefe685c-4b3f-4318-a1ea-8497c774326c"/>
@@ -4683,21 +4717,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="890b14a5-ed4a-422d-85a5-a10e9e237f7d">
-      <UserInfo>
-        <DisplayName>Ross Walker</DisplayName>
-        <AccountId>22</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC761B82-E96C-46F8-BDA5-C1773C8865DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="890b14a5-ed4a-422d-85a5-a10e9e237f7d"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="fefe685c-4b3f-4318-a1ea-8497c774326c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9154765-C794-4067-A64A-ACA6EA7134EB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -4705,7 +4742,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52D3CBED-BF76-433F-94D3-DB991E5749CF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4722,21 +4759,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC761B82-E96C-46F8-BDA5-C1773C8865DE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="fefe685c-4b3f-4318-a1ea-8497c774326c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="890b14a5-ed4a-422d-85a5-a10e9e237f7d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>